<commit_message>
Auf dem REFs ans Laufen zu bekommen. Es entstehen leider noch zeitfensterunzulässige Lösungen.
</commit_message>
<xml_diff>
--- a/output/localSearch 2015-01-28-20-26-30.xlsx
+++ b/output/localSearch 2015-01-28-20-26-30.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="localSearch 2015-01-28-20-26-30" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Problem</t>
   </si>
@@ -40,9 +40,6 @@
     <t>C101</t>
   </si>
   <si>
-    <t>828.94</t>
-  </si>
-  <si>
     <t>C102</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
     <t>C104</t>
   </si>
   <si>
-    <t>824.78</t>
-  </si>
-  <si>
     <t>C105</t>
   </si>
   <si>
@@ -76,271 +70,142 @@
     <t>C202</t>
   </si>
   <si>
-    <t>591.56</t>
-  </si>
-  <si>
     <t>C203</t>
   </si>
   <si>
     <t>C204</t>
   </si>
   <si>
-    <t>591.17</t>
-  </si>
-  <si>
     <t>C205</t>
   </si>
   <si>
-    <t>590.6</t>
-  </si>
-  <si>
     <t>C206</t>
   </si>
   <si>
-    <t>588.29</t>
-  </si>
-  <si>
     <t>C207</t>
   </si>
   <si>
-    <t>588.49</t>
-  </si>
-  <si>
     <t>C208</t>
   </si>
   <si>
     <t>R101</t>
   </si>
   <si>
-    <t>588.32</t>
-  </si>
-  <si>
     <t>R102</t>
   </si>
   <si>
-    <t>1650.8</t>
-  </si>
-  <si>
     <t>R103</t>
   </si>
   <si>
-    <t>1486.12</t>
-  </si>
-  <si>
     <t>R104</t>
   </si>
   <si>
-    <t>1292.68</t>
-  </si>
-  <si>
     <t>R105</t>
   </si>
   <si>
-    <t>1007.31</t>
-  </si>
-  <si>
     <t>R106</t>
   </si>
   <si>
-    <t>1377.11</t>
-  </si>
-  <si>
     <t>R107</t>
   </si>
   <si>
-    <t>1252.03</t>
-  </si>
-  <si>
     <t>R108</t>
   </si>
   <si>
-    <t>1104.66</t>
-  </si>
-  <si>
     <t>R109</t>
   </si>
   <si>
-    <t>960.88</t>
-  </si>
-  <si>
     <t>R110</t>
   </si>
   <si>
-    <t>1194.73</t>
-  </si>
-  <si>
     <t>R111</t>
   </si>
   <si>
-    <t>1118.84</t>
-  </si>
-  <si>
     <t>R112</t>
   </si>
   <si>
-    <t>1096.72</t>
-  </si>
-  <si>
     <t>R201</t>
   </si>
   <si>
-    <t>982.14</t>
-  </si>
-  <si>
     <t>R202</t>
   </si>
   <si>
-    <t>1252.37</t>
-  </si>
-  <si>
     <t>R203</t>
   </si>
   <si>
-    <t>1191.7</t>
-  </si>
-  <si>
     <t>R204</t>
   </si>
   <si>
-    <t>939.5</t>
-  </si>
-  <si>
     <t>R205</t>
   </si>
   <si>
-    <t>825.52</t>
-  </si>
-  <si>
     <t>R206</t>
   </si>
   <si>
-    <t>994.42</t>
-  </si>
-  <si>
     <t>R207</t>
   </si>
   <si>
-    <t>906.14</t>
-  </si>
-  <si>
     <t>R208</t>
   </si>
   <si>
-    <t>890.61</t>
-  </si>
-  <si>
     <t>R209</t>
   </si>
   <si>
-    <t>726.82</t>
-  </si>
-  <si>
     <t>R210</t>
   </si>
   <si>
-    <t>909.16</t>
-  </si>
-  <si>
     <t>R211</t>
   </si>
   <si>
-    <t>939.37</t>
-  </si>
-  <si>
     <t>RC101</t>
   </si>
   <si>
-    <t>885.71</t>
-  </si>
-  <si>
     <t>RC102</t>
   </si>
   <si>
-    <t>1696.94</t>
-  </si>
-  <si>
     <t>RC103</t>
   </si>
   <si>
-    <t>1554.75</t>
-  </si>
-  <si>
     <t>RC104</t>
   </si>
   <si>
-    <t>1261.67</t>
-  </si>
-  <si>
     <t>RC105</t>
   </si>
   <si>
-    <t>1135.48</t>
-  </si>
-  <si>
     <t>RC106</t>
   </si>
   <si>
-    <t>1629.44</t>
-  </si>
-  <si>
     <t>RC107</t>
   </si>
   <si>
-    <t>1424.73</t>
-  </si>
-  <si>
     <t>RC108</t>
   </si>
   <si>
-    <t>1230.48</t>
-  </si>
-  <si>
     <t>RC201</t>
   </si>
   <si>
-    <t>1139.82</t>
-  </si>
-  <si>
     <t>RC202</t>
   </si>
   <si>
-    <t>1406.94</t>
-  </si>
-  <si>
     <t>RC203</t>
   </si>
   <si>
-    <t>1365.65</t>
-  </si>
-  <si>
     <t>RC204</t>
   </si>
   <si>
-    <t>1049.62</t>
-  </si>
-  <si>
     <t>RC205</t>
   </si>
   <si>
-    <t>798.46</t>
-  </si>
-  <si>
     <t>RC206</t>
   </si>
   <si>
-    <t>1297.65</t>
-  </si>
-  <si>
     <t>RC207</t>
   </si>
   <si>
-    <t>1146.32</t>
-  </si>
-  <si>
     <t>RC208</t>
   </si>
   <si>
-    <t>1061.14</t>
+    <t>Local Search besser als bester bekannter Wert?</t>
   </si>
 </sst>
 </file>
@@ -1169,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1049,7 @@
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1206,8 +1071,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1223,16 +1091,20 @@
       <c r="E2">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="F2">
+        <v>828.94</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f>IF(D2&lt;F2,IF(E2&lt;=G2,"Ja","Nein"),"Nein")</f>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>5598.4110000000001</v>
@@ -1246,16 +1118,20 @@
       <c r="E3">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
+      <c r="F3">
+        <v>828.94</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H57" si="0">IF(D3&lt;F3,IF(E3&lt;=G3,"Ja","Nein"),"Nein")</f>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>5484.4290000000001</v>
@@ -1269,16 +1145,20 @@
       <c r="E4">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
+      <c r="F4">
+        <v>828.94</v>
       </c>
       <c r="G4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>5399.4979999999996</v>
@@ -1292,16 +1172,20 @@
       <c r="E5">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
-        <v>12</v>
+      <c r="F5">
+        <v>824.78</v>
       </c>
       <c r="G5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>5425.8540000000003</v>
@@ -1315,16 +1199,20 @@
       <c r="E6">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
-        <v>8</v>
+      <c r="F6">
+        <v>828.94</v>
       </c>
       <c r="G6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>5425.8540000000003</v>
@@ -1338,16 +1226,20 @@
       <c r="E7">
         <v>10</v>
       </c>
-      <c r="F7" t="s">
-        <v>8</v>
+      <c r="F7">
+        <v>828.94</v>
       </c>
       <c r="G7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>5546.4570000000003</v>
@@ -1361,16 +1253,20 @@
       <c r="E8">
         <v>10</v>
       </c>
-      <c r="F8" t="s">
-        <v>8</v>
+      <c r="F8">
+        <v>828.94</v>
       </c>
       <c r="G8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>5546.4570000000003</v>
@@ -1384,16 +1280,20 @@
       <c r="E9">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
-        <v>8</v>
+      <c r="F9">
+        <v>828.94</v>
       </c>
       <c r="G9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>5371.1049999999996</v>
@@ -1407,16 +1307,20 @@
       <c r="E10">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
+      <c r="F10">
+        <v>828.94</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>5579.0140000000001</v>
@@ -1430,16 +1334,20 @@
       <c r="E11">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
-        <v>8</v>
+      <c r="F11">
+        <v>828.94</v>
       </c>
       <c r="G11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>5440.03</v>
@@ -1453,16 +1361,20 @@
       <c r="E12">
         <v>3</v>
       </c>
-      <c r="F12" t="s">
-        <v>20</v>
+      <c r="F12">
+        <v>591.55999999999995</v>
       </c>
       <c r="G12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>5350.9570000000003</v>
@@ -1476,16 +1388,20 @@
       <c r="E13">
         <v>5</v>
       </c>
-      <c r="F13" t="s">
-        <v>20</v>
+      <c r="F13">
+        <v>591.55999999999995</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>5129.04</v>
@@ -1499,16 +1415,20 @@
       <c r="E14">
         <v>5</v>
       </c>
-      <c r="F14" t="s">
-        <v>23</v>
+      <c r="F14">
+        <v>591.16999999999996</v>
       </c>
       <c r="G14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>5503.9459999999999</v>
@@ -1522,16 +1442,20 @@
       <c r="E15">
         <v>3</v>
       </c>
-      <c r="F15" t="s">
-        <v>25</v>
+      <c r="F15">
+        <v>590.6</v>
       </c>
       <c r="G15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>Ja</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>5397.0910000000003</v>
@@ -1545,16 +1469,20 @@
       <c r="E16">
         <v>7</v>
       </c>
-      <c r="F16" t="s">
-        <v>27</v>
+      <c r="F16">
+        <v>588.29</v>
       </c>
       <c r="G16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>4888.6660000000002</v>
@@ -1568,16 +1496,20 @@
       <c r="E17">
         <v>4</v>
       </c>
-      <c r="F17" t="s">
-        <v>29</v>
+      <c r="F17">
+        <v>588.49</v>
       </c>
       <c r="G17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>5345.3459999999995</v>
@@ -1591,16 +1523,20 @@
       <c r="E18">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
-        <v>27</v>
+      <c r="F18">
+        <v>588.29</v>
       </c>
       <c r="G18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>4877.2079999999996</v>
@@ -1614,16 +1550,20 @@
       <c r="E19">
         <v>25</v>
       </c>
-      <c r="F19" t="s">
-        <v>32</v>
+      <c r="F19">
+        <v>588.32000000000005</v>
       </c>
       <c r="G19">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>4823.9840000000004</v>
@@ -1637,16 +1577,20 @@
       <c r="E20">
         <v>21</v>
       </c>
-      <c r="F20" t="s">
-        <v>34</v>
+      <c r="F20">
+        <v>1650.8</v>
       </c>
       <c r="G20">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>4796.8450000000003</v>
@@ -1660,16 +1604,20 @@
       <c r="E21">
         <v>16</v>
       </c>
-      <c r="F21" t="s">
-        <v>36</v>
+      <c r="F21">
+        <v>1486.12</v>
       </c>
       <c r="G21">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>4835.7370000000001</v>
@@ -1683,16 +1631,20 @@
       <c r="E22">
         <v>13</v>
       </c>
-      <c r="F22" t="s">
-        <v>38</v>
+      <c r="F22">
+        <v>1292.68</v>
       </c>
       <c r="G22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>4877.0749999999998</v>
@@ -1706,16 +1658,20 @@
       <c r="E23">
         <v>19</v>
       </c>
-      <c r="F23" t="s">
-        <v>40</v>
+      <c r="F23">
+        <v>1007.31</v>
       </c>
       <c r="G23">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>4797.991</v>
@@ -1729,16 +1685,20 @@
       <c r="E24">
         <v>14</v>
       </c>
-      <c r="F24" t="s">
-        <v>42</v>
+      <c r="F24">
+        <v>1377.11</v>
       </c>
       <c r="G24">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>4750.9589999999998</v>
@@ -1752,16 +1712,20 @@
       <c r="E25">
         <v>13</v>
       </c>
-      <c r="F25" t="s">
-        <v>44</v>
+      <c r="F25">
+        <v>1252.03</v>
       </c>
       <c r="G25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>4800.7389999999996</v>
@@ -1775,16 +1739,20 @@
       <c r="E26">
         <v>13</v>
       </c>
-      <c r="F26" t="s">
-        <v>46</v>
+      <c r="F26">
+        <v>1104.6600000000001</v>
       </c>
       <c r="G26">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>4806.9279999999999</v>
@@ -1798,16 +1766,20 @@
       <c r="E27">
         <v>16</v>
       </c>
-      <c r="F27" t="s">
-        <v>48</v>
+      <c r="F27">
+        <v>960.88</v>
       </c>
       <c r="G27">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>4827.0959999999995</v>
@@ -1821,16 +1793,20 @@
       <c r="E28">
         <v>14</v>
       </c>
-      <c r="F28" t="s">
-        <v>50</v>
+      <c r="F28">
+        <v>1194.73</v>
       </c>
       <c r="G28">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>4718.085</v>
@@ -1844,16 +1820,20 @@
       <c r="E29">
         <v>13</v>
       </c>
-      <c r="F29" t="s">
-        <v>52</v>
+      <c r="F29">
+        <v>1118.8399999999999</v>
       </c>
       <c r="G29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>4685.2349999999997</v>
@@ -1867,16 +1847,20 @@
       <c r="E30">
         <v>11</v>
       </c>
-      <c r="F30" t="s">
-        <v>54</v>
+      <c r="F30">
+        <v>1096.72</v>
       </c>
       <c r="G30">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>4612.9210000000003</v>
@@ -1890,16 +1874,20 @@
       <c r="E31">
         <v>13</v>
       </c>
-      <c r="F31" t="s">
-        <v>56</v>
+      <c r="F31">
+        <v>982.14</v>
       </c>
       <c r="G31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>4618.2380000000003</v>
@@ -1913,16 +1901,20 @@
       <c r="E32">
         <v>11</v>
       </c>
-      <c r="F32" t="s">
-        <v>58</v>
+      <c r="F32">
+        <v>1252.3699999999999</v>
       </c>
       <c r="G32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B33">
         <v>4489.95</v>
@@ -1936,16 +1928,20 @@
       <c r="E33">
         <v>8</v>
       </c>
-      <c r="F33" t="s">
-        <v>60</v>
+      <c r="F33">
+        <v>1191.7</v>
       </c>
       <c r="G33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <v>4435.9390000000003</v>
@@ -1959,16 +1955,20 @@
       <c r="E34">
         <v>6</v>
       </c>
-      <c r="F34" t="s">
-        <v>62</v>
+      <c r="F34">
+        <v>939.5</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>4394.3789999999999</v>
@@ -1982,16 +1982,20 @@
       <c r="E35">
         <v>8</v>
       </c>
-      <c r="F35" t="s">
-        <v>64</v>
+      <c r="F35">
+        <v>825.52</v>
       </c>
       <c r="G35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>4285.3379999999997</v>
@@ -2005,16 +2009,20 @@
       <c r="E36">
         <v>10</v>
       </c>
-      <c r="F36" t="s">
-        <v>66</v>
+      <c r="F36">
+        <v>994.42</v>
       </c>
       <c r="G36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>4202.6059999999998</v>
@@ -2028,16 +2036,20 @@
       <c r="E37">
         <v>5</v>
       </c>
-      <c r="F37" t="s">
-        <v>68</v>
+      <c r="F37">
+        <v>906.14</v>
       </c>
       <c r="G37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>4046.59</v>
@@ -2051,16 +2063,20 @@
       <c r="E38">
         <v>4</v>
       </c>
-      <c r="F38" t="s">
-        <v>70</v>
+      <c r="F38">
+        <v>890.61</v>
       </c>
       <c r="G38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="B39">
         <v>4177.5360000000001</v>
@@ -2074,16 +2090,20 @@
       <c r="E39">
         <v>8</v>
       </c>
-      <c r="F39" t="s">
-        <v>72</v>
+      <c r="F39">
+        <v>726.82</v>
       </c>
       <c r="G39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B40">
         <v>4550.0230000000001</v>
@@ -2097,16 +2117,20 @@
       <c r="E40">
         <v>9</v>
       </c>
-      <c r="F40" t="s">
-        <v>74</v>
+      <c r="F40">
+        <v>909.16</v>
       </c>
       <c r="G40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="B41">
         <v>3783.4940000000001</v>
@@ -2120,16 +2144,20 @@
       <c r="E41">
         <v>7</v>
       </c>
-      <c r="F41" t="s">
-        <v>76</v>
+      <c r="F41">
+        <v>939.37</v>
       </c>
       <c r="G41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="B42">
         <v>6498.1580000000004</v>
@@ -2143,16 +2171,20 @@
       <c r="E42">
         <v>18</v>
       </c>
-      <c r="F42" t="s">
-        <v>78</v>
+      <c r="F42">
+        <v>885.71</v>
       </c>
       <c r="G42">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="B43">
         <v>6483.8860000000004</v>
@@ -2166,16 +2198,20 @@
       <c r="E43">
         <v>16</v>
       </c>
-      <c r="F43" t="s">
-        <v>80</v>
+      <c r="F43">
+        <v>1696.94</v>
       </c>
       <c r="G43">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="B44">
         <v>6462.3360000000002</v>
@@ -2189,16 +2225,20 @@
       <c r="E44">
         <v>15</v>
       </c>
-      <c r="F44" t="s">
-        <v>82</v>
+      <c r="F44">
+        <v>1554.75</v>
       </c>
       <c r="G44">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="B45">
         <v>6347.6459999999997</v>
@@ -2212,16 +2252,20 @@
       <c r="E45">
         <v>12</v>
       </c>
-      <c r="F45" t="s">
-        <v>84</v>
+      <c r="F45">
+        <v>1261.67</v>
       </c>
       <c r="G45">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="B46">
         <v>6483.8860000000004</v>
@@ -2235,16 +2279,20 @@
       <c r="E46">
         <v>20</v>
       </c>
-      <c r="F46" t="s">
-        <v>86</v>
+      <c r="F46">
+        <v>1135.48</v>
       </c>
       <c r="G46">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="B47">
         <v>6491.0159999999996</v>
@@ -2258,16 +2306,20 @@
       <c r="E47">
         <v>16</v>
       </c>
-      <c r="F47" t="s">
-        <v>88</v>
+      <c r="F47">
+        <v>1629.44</v>
       </c>
       <c r="G47">
         <v>11</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="B48">
         <v>6420.8519999999999</v>
@@ -2281,16 +2333,20 @@
       <c r="E48">
         <v>13</v>
       </c>
-      <c r="F48" t="s">
-        <v>90</v>
+      <c r="F48">
+        <v>1424.73</v>
       </c>
       <c r="G48">
         <v>11</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="B49">
         <v>6475.951</v>
@@ -2304,16 +2360,20 @@
       <c r="E49">
         <v>12</v>
       </c>
-      <c r="F49" t="s">
-        <v>92</v>
+      <c r="F49">
+        <v>1230.48</v>
       </c>
       <c r="G49">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B50">
         <v>6215.8710000000001</v>
@@ -2327,16 +2387,20 @@
       <c r="E50">
         <v>13</v>
       </c>
-      <c r="F50" t="s">
-        <v>94</v>
+      <c r="F50">
+        <v>1139.82</v>
       </c>
       <c r="G50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="B51">
         <v>5975.0720000000001</v>
@@ -2350,16 +2414,20 @@
       <c r="E51">
         <v>13</v>
       </c>
-      <c r="F51" t="s">
-        <v>96</v>
+      <c r="F51">
+        <v>1406.94</v>
       </c>
       <c r="G51">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="B52">
         <v>5894.1210000000001</v>
@@ -2373,16 +2441,20 @@
       <c r="E52">
         <v>8</v>
       </c>
-      <c r="F52" t="s">
-        <v>98</v>
+      <c r="F52">
+        <v>1365.65</v>
       </c>
       <c r="G52">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="B53">
         <v>4913.2120000000004</v>
@@ -2396,16 +2468,20 @@
       <c r="E53">
         <v>6</v>
       </c>
-      <c r="F53" t="s">
-        <v>100</v>
+      <c r="F53">
+        <v>1049.6199999999999</v>
       </c>
       <c r="G53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="B54">
         <v>6047.701</v>
@@ -2419,16 +2495,20 @@
       <c r="E54">
         <v>12</v>
       </c>
-      <c r="F54" t="s">
-        <v>102</v>
+      <c r="F54">
+        <v>798.46</v>
       </c>
       <c r="G54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>5735.4160000000002</v>
@@ -2442,16 +2522,20 @@
       <c r="E55">
         <v>11</v>
       </c>
-      <c r="F55" t="s">
-        <v>104</v>
+      <c r="F55">
+        <v>1297.6500000000001</v>
       </c>
       <c r="G55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="B56">
         <v>5811.7560000000003</v>
@@ -2465,16 +2549,20 @@
       <c r="E56">
         <v>8</v>
       </c>
-      <c r="F56" t="s">
-        <v>106</v>
+      <c r="F56">
+        <v>1146.32</v>
       </c>
       <c r="G56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="B57">
         <v>5510.6289999999999</v>
@@ -2488,11 +2576,15 @@
       <c r="E57">
         <v>6</v>
       </c>
-      <c r="F57" t="s">
-        <v>108</v>
+      <c r="F57">
+        <v>1061.1400000000001</v>
       </c>
       <c r="G57">
         <v>3</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="0"/>
+        <v>Nein</v>
       </c>
     </row>
   </sheetData>

</xml_diff>